<commit_message>
JSON in Some Pages and Footer
- JS, JSON and HTML Complete for index.html
- JS, JSON and HTML Complete for goal1.html
- JS, JSON and HTML Complete for goal2.html
- JS, JSON and HTML Complete for goal3.html
- Footer Implemented into Backend
</commit_message>
<xml_diff>
--- a/documentation/Code Record.xlsx
+++ b/documentation/Code Record.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28129"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11110"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\panka\OneDrive\Documents\GitHub\CMP4011A\documentation\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/aff6c2e7aaf478e0/Documents/University Files/Modules/CMP4011A/Lab Work/Group Project/CMP4011A/documentation/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D74FA308-836D-4033-A6E1-6751CCCB6D26}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="11" documentId="13_ncr:1_{D74FA308-836D-4033-A6E1-6751CCCB6D26}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{BD9A1D04-B8EB-1B42-B3F9-DD9B263212E8}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{080229FA-A9D9-E748-BB1E-E732181A4591}"/>
+    <workbookView xWindow="0" yWindow="740" windowWidth="23260" windowHeight="12460" xr2:uid="{080229FA-A9D9-E748-BB1E-E732181A4591}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="93" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="96" uniqueCount="26">
   <si>
     <t>Task</t>
   </si>
@@ -593,28 +593,28 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8E770589-ABF5-1D4F-B841-D2FC3B293113}">
   <dimension ref="A1:J36"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A15" zoomScale="125" workbookViewId="0">
-      <selection activeCell="D11" sqref="D11"/>
+    <sheetView tabSelected="1" topLeftCell="A5" zoomScale="125" workbookViewId="0">
+      <selection activeCell="G14" sqref="G14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.19921875" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.1640625" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="5.296875" customWidth="1"/>
+    <col min="1" max="1" width="5.33203125" customWidth="1"/>
     <col min="2" max="2" width="14" customWidth="1"/>
-    <col min="3" max="3" width="11.796875" customWidth="1"/>
+    <col min="3" max="3" width="11.83203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" ht="19.05" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:4" ht="19" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="1"/>
     </row>
-    <row r="2" spans="1:4" ht="43.05" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:4" ht="43" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B2" s="12" t="s">
         <v>18</v>
       </c>
       <c r="C2" s="12"/>
       <c r="D2" s="12"/>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B4" s="3" t="s">
         <v>12</v>
       </c>
@@ -625,7 +625,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B5" s="2" t="s">
         <v>2</v>
       </c>
@@ -636,7 +636,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B6" s="2" t="s">
         <v>2</v>
       </c>
@@ -647,7 +647,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B7" s="2" t="s">
         <v>2</v>
       </c>
@@ -658,7 +658,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B8" s="2" t="s">
         <v>2</v>
       </c>
@@ -669,7 +669,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B9" s="2" t="s">
         <v>3</v>
       </c>
@@ -680,7 +680,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B10" s="2" t="s">
         <v>3</v>
       </c>
@@ -691,16 +691,18 @@
         <v>10</v>
       </c>
     </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B11" s="2" t="s">
         <v>3</v>
       </c>
       <c r="C11" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="D11" s="4"/>
-    </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="D11" s="4" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B12" s="2" t="s">
         <v>3</v>
       </c>
@@ -711,7 +713,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B13" s="2" t="s">
         <v>4</v>
       </c>
@@ -722,7 +724,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B14" s="2" t="s">
         <v>4</v>
       </c>
@@ -733,16 +735,18 @@
         <v>10</v>
       </c>
     </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B15" s="2" t="s">
         <v>4</v>
       </c>
       <c r="C15" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="D15" s="4"/>
-    </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="D15" s="4" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B16" s="2" t="s">
         <v>4</v>
       </c>
@@ -753,7 +757,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="17" spans="2:10" x14ac:dyDescent="0.3">
+    <row r="17" spans="2:10" x14ac:dyDescent="0.2">
       <c r="B17" s="2" t="s">
         <v>8</v>
       </c>
@@ -764,7 +768,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="18" spans="2:10" x14ac:dyDescent="0.3">
+    <row r="18" spans="2:10" x14ac:dyDescent="0.2">
       <c r="B18" s="2" t="s">
         <v>8</v>
       </c>
@@ -775,16 +779,18 @@
         <v>10</v>
       </c>
     </row>
-    <row r="19" spans="2:10" x14ac:dyDescent="0.3">
+    <row r="19" spans="2:10" x14ac:dyDescent="0.2">
       <c r="B19" s="2" t="s">
         <v>8</v>
       </c>
       <c r="C19" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="D19" s="4"/>
-    </row>
-    <row r="20" spans="2:10" x14ac:dyDescent="0.3">
+      <c r="D19" s="4" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="20" spans="2:10" x14ac:dyDescent="0.2">
       <c r="B20" s="2" t="s">
         <v>8</v>
       </c>
@@ -795,7 +801,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="21" spans="2:10" x14ac:dyDescent="0.3">
+    <row r="21" spans="2:10" x14ac:dyDescent="0.2">
       <c r="B21" s="2" t="s">
         <v>14</v>
       </c>
@@ -806,7 +812,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="22" spans="2:10" x14ac:dyDescent="0.3">
+    <row r="22" spans="2:10" x14ac:dyDescent="0.2">
       <c r="B22" s="2" t="s">
         <v>14</v>
       </c>
@@ -817,7 +823,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="23" spans="2:10" x14ac:dyDescent="0.3">
+    <row r="23" spans="2:10" x14ac:dyDescent="0.2">
       <c r="B23" s="2" t="s">
         <v>14</v>
       </c>
@@ -828,7 +834,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="24" spans="2:10" x14ac:dyDescent="0.3">
+    <row r="24" spans="2:10" x14ac:dyDescent="0.2">
       <c r="B24" s="2" t="s">
         <v>14</v>
       </c>
@@ -839,7 +845,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="25" spans="2:10" x14ac:dyDescent="0.3">
+    <row r="25" spans="2:10" x14ac:dyDescent="0.2">
       <c r="B25" s="2" t="s">
         <v>15</v>
       </c>
@@ -850,7 +856,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="26" spans="2:10" x14ac:dyDescent="0.3">
+    <row r="26" spans="2:10" x14ac:dyDescent="0.2">
       <c r="B26" s="2" t="s">
         <v>15</v>
       </c>
@@ -861,7 +867,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="27" spans="2:10" x14ac:dyDescent="0.3">
+    <row r="27" spans="2:10" x14ac:dyDescent="0.2">
       <c r="B27" s="2" t="s">
         <v>15</v>
       </c>
@@ -875,7 +881,7 @@
       <c r="I27" s="11"/>
       <c r="J27" s="11"/>
     </row>
-    <row r="28" spans="2:10" x14ac:dyDescent="0.3">
+    <row r="28" spans="2:10" x14ac:dyDescent="0.2">
       <c r="B28" s="2" t="s">
         <v>15</v>
       </c>
@@ -889,7 +895,7 @@
       <c r="I28" s="11"/>
       <c r="J28" s="11"/>
     </row>
-    <row r="29" spans="2:10" x14ac:dyDescent="0.3">
+    <row r="29" spans="2:10" x14ac:dyDescent="0.2">
       <c r="B29" s="2" t="s">
         <v>15</v>
       </c>
@@ -903,7 +909,7 @@
       <c r="I29" s="11"/>
       <c r="J29" s="11"/>
     </row>
-    <row r="30" spans="2:10" x14ac:dyDescent="0.3">
+    <row r="30" spans="2:10" x14ac:dyDescent="0.2">
       <c r="B30" s="5" t="s">
         <v>17</v>
       </c>
@@ -917,7 +923,7 @@
       <c r="I30" s="11"/>
       <c r="J30" s="11"/>
     </row>
-    <row r="31" spans="2:10" x14ac:dyDescent="0.3">
+    <row r="31" spans="2:10" x14ac:dyDescent="0.2">
       <c r="B31" s="5" t="s">
         <v>17</v>
       </c>
@@ -928,7 +934,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="32" spans="2:10" x14ac:dyDescent="0.3">
+    <row r="32" spans="2:10" x14ac:dyDescent="0.2">
       <c r="B32" s="5" t="s">
         <v>17</v>
       </c>
@@ -939,7 +945,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="33" spans="2:4" x14ac:dyDescent="0.3">
+    <row r="33" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B33" s="5" t="s">
         <v>17</v>
       </c>
@@ -950,7 +956,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="34" spans="2:4" x14ac:dyDescent="0.3">
+    <row r="34" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B34" s="9" t="s">
         <v>20</v>
       </c>
@@ -961,7 +967,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="36" spans="2:4" x14ac:dyDescent="0.3">
+    <row r="36" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B36" s="13" t="s">
         <v>16</v>
       </c>

</xml_diff>